<commit_message>
added ligands that were excluded
</commit_message>
<xml_diff>
--- a/benchmarking/Benchmarking_Dataset.xlsx
+++ b/benchmarking/Benchmarking_Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiojeong/Documents/ligify-reverse-1/benchmarking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEC150C-D78B-354B-96CD-F5624036EDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2400505E-2ED8-9A42-9254-348B31A9F4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1727" uniqueCount="659">
   <si>
     <t>Chemical name</t>
   </si>
@@ -1904,9 +1904,6 @@
     <t>true ligand NOT within top 5 returned chemicals</t>
   </si>
   <si>
-    <t>total fails</t>
-  </si>
-  <si>
     <t>invalid refseq</t>
   </si>
   <si>
@@ -2010,13 +2007,16 @@
   </si>
   <si>
     <t>3-methyl-2-oxobutanoate</t>
+  </si>
+  <si>
+    <t>failures</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2154,8 +2154,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="7"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2171,6 +2183,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2196,7 +2214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2228,9 +2246,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2246,6 +2262,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -2468,8 +2490,8 @@
   </sheetPr>
   <dimension ref="A1:AJ141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T71" zoomScale="75" workbookViewId="0">
-      <selection activeCell="W106" sqref="W106"/>
+    <sheetView tabSelected="1" topLeftCell="K37" zoomScale="63" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2488,14 +2510,16 @@
     <col min="14" max="14" width="8.1640625" customWidth="1"/>
     <col min="19" max="19" width="35.5" customWidth="1"/>
     <col min="20" max="20" width="36" style="16" customWidth="1"/>
-    <col min="21" max="21" width="29.5" style="31" customWidth="1"/>
+    <col min="21" max="21" width="29.5" style="29" customWidth="1"/>
     <col min="22" max="22" width="29.5" customWidth="1"/>
     <col min="23" max="23" width="22.6640625" customWidth="1"/>
     <col min="24" max="24" width="18.6640625" customWidth="1"/>
     <col min="25" max="25" width="50.5" style="14" customWidth="1"/>
     <col min="26" max="26" width="23" style="14" customWidth="1"/>
-    <col min="27" max="27" width="72" style="27" customWidth="1"/>
-    <col min="28" max="33" width="12.6640625" style="14"/>
+    <col min="27" max="27" width="72" style="25" customWidth="1"/>
+    <col min="28" max="28" width="12.6640625" style="14"/>
+    <col min="29" max="29" width="14.1640625" customWidth="1"/>
+    <col min="30" max="33" width="12.6640625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2557,7 +2581,7 @@
       <c r="T1" s="12" t="s">
         <v>593</v>
       </c>
-      <c r="U1" s="30" t="s">
+      <c r="U1" s="28" t="s">
         <v>594</v>
       </c>
       <c r="V1" s="12" t="s">
@@ -2573,15 +2597,17 @@
         <v>599</v>
       </c>
       <c r="Z1" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="AA1" s="24" t="s">
         <v>626</v>
       </c>
-      <c r="AA1" s="26" t="s">
-        <v>627</v>
-      </c>
       <c r="AB1" s="9" t="s">
-        <v>625</v>
-      </c>
-      <c r="AC1" s="9"/>
+        <v>624</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AD1" s="4"/>
       <c r="AE1" s="4"/>
       <c r="AF1" s="4"/>
@@ -2642,7 +2668,7 @@
       <c r="T2" s="13">
         <v>86.385563636363599</v>
       </c>
-      <c r="U2" s="27" t="s">
+      <c r="U2" s="25" t="s">
         <v>595</v>
       </c>
       <c r="X2" s="13" t="s">
@@ -2650,9 +2676,11 @@
       </c>
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
-      <c r="AA2" s="26"/>
+      <c r="AA2" s="24"/>
       <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
+      <c r="AC2" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="AD2" s="4"/>
       <c r="AE2" s="4"/>
       <c r="AF2" s="4"/>
@@ -2713,7 +2741,7 @@
       <c r="T3" s="18">
         <v>87.758733333333296</v>
       </c>
-      <c r="U3" s="27" t="s">
+      <c r="U3" s="25" t="s">
         <v>596</v>
       </c>
       <c r="W3" s="2"/>
@@ -2722,9 +2750,11 @@
       </c>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
-      <c r="AA3" s="26"/>
+      <c r="AA3" s="24"/>
       <c r="AB3" s="4"/>
-      <c r="AC3" s="4"/>
+      <c r="AC3" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="AD3" s="4"/>
       <c r="AE3" s="4"/>
       <c r="AF3" s="4"/>
@@ -2787,7 +2817,7 @@
       <c r="T4" s="18">
         <v>86.764866666666606</v>
       </c>
-      <c r="U4" s="27" t="s">
+      <c r="U4" s="25" t="s">
         <v>595</v>
       </c>
       <c r="W4" s="2"/>
@@ -2796,9 +2826,11 @@
       </c>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
-      <c r="AA4" s="26"/>
+      <c r="AA4" s="24"/>
       <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
+      <c r="AC4" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AD4" s="4"/>
       <c r="AE4" s="4"/>
       <c r="AF4" s="4"/>
@@ -2861,7 +2893,7 @@
       <c r="T5" s="18">
         <v>92.667487499999993</v>
       </c>
-      <c r="U5" s="27" t="s">
+      <c r="U5" s="25" t="s">
         <v>595</v>
       </c>
       <c r="W5" s="2"/>
@@ -2870,9 +2902,11 @@
       </c>
       <c r="Y5" s="4"/>
       <c r="Z5" s="4"/>
-      <c r="AA5" s="26"/>
+      <c r="AA5" s="24"/>
       <c r="AB5" s="4"/>
-      <c r="AC5" s="4"/>
+      <c r="AC5" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AD5" s="4"/>
       <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
@@ -2933,7 +2967,7 @@
       <c r="T6" s="18">
         <v>94.259541666666607</v>
       </c>
-      <c r="U6" s="27" t="s">
+      <c r="U6" s="25" t="s">
         <v>595</v>
       </c>
       <c r="W6" s="2"/>
@@ -2942,9 +2976,11 @@
       </c>
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
-      <c r="AA6" s="26"/>
+      <c r="AA6" s="24"/>
       <c r="AB6" s="4"/>
-      <c r="AC6" s="4"/>
+      <c r="AC6" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="AD6" s="4"/>
       <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
@@ -3005,7 +3041,7 @@
       <c r="T7" s="18">
         <v>84.385515151515094</v>
       </c>
-      <c r="U7" s="27" t="s">
+      <c r="U7" s="25" t="s">
         <v>596</v>
       </c>
       <c r="W7" s="2"/>
@@ -3014,9 +3050,11 @@
       </c>
       <c r="Y7" s="4"/>
       <c r="Z7" s="4"/>
-      <c r="AA7" s="26"/>
+      <c r="AA7" s="24"/>
       <c r="AB7" s="4"/>
-      <c r="AC7" s="4"/>
+      <c r="AC7" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
@@ -3077,7 +3115,7 @@
       <c r="T8" s="18">
         <v>87.926316666666594</v>
       </c>
-      <c r="U8" s="27" t="s">
+      <c r="U8" s="25" t="s">
         <v>597</v>
       </c>
       <c r="W8" s="2"/>
@@ -3086,9 +3124,11 @@
       </c>
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
-      <c r="AA8" s="26"/>
+      <c r="AA8" s="24"/>
       <c r="AB8" s="4"/>
-      <c r="AC8" s="4"/>
+      <c r="AC8" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="AD8" s="4"/>
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
@@ -3151,7 +3191,7 @@
       <c r="T9" s="18">
         <v>81.1666666666666</v>
       </c>
-      <c r="U9" s="27" t="s">
+      <c r="U9" s="25" t="s">
         <v>598</v>
       </c>
       <c r="W9" s="2"/>
@@ -3160,9 +3200,11 @@
       </c>
       <c r="Y9" s="4"/>
       <c r="Z9" s="4"/>
-      <c r="AA9" s="26"/>
+      <c r="AA9" s="24"/>
       <c r="AB9" s="4"/>
-      <c r="AC9" s="4"/>
+      <c r="AC9" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="AD9" s="4"/>
       <c r="AE9" s="4"/>
       <c r="AF9" s="4"/>
@@ -3225,7 +3267,7 @@
       <c r="T10" s="22">
         <v>90.275434782608599</v>
       </c>
-      <c r="U10" s="27" t="s">
+      <c r="U10" s="25" t="s">
         <v>597</v>
       </c>
       <c r="V10" s="14"/>
@@ -3233,13 +3275,15 @@
       <c r="X10" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Y10" s="25" t="s">
+      <c r="Y10" s="4" t="s">
         <v>600</v>
       </c>
       <c r="Z10" s="4"/>
-      <c r="AA10" s="26"/>
-      <c r="AB10" s="25"/>
-      <c r="AC10" s="4"/>
+      <c r="AA10" s="24"/>
+      <c r="AB10" s="4"/>
+      <c r="AC10" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="AD10" s="4"/>
       <c r="AE10" s="4"/>
       <c r="AF10" s="4"/>
@@ -3302,18 +3346,20 @@
       <c r="T11" s="18">
         <v>93.935837202380895</v>
       </c>
-      <c r="U11" s="27" t="s">
+      <c r="U11" s="25" t="s">
         <v>601</v>
       </c>
       <c r="W11" s="2"/>
       <c r="X11" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="Y11" s="25"/>
+      <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
-      <c r="AA11" s="26"/>
+      <c r="AA11" s="24"/>
       <c r="AB11" s="4"/>
-      <c r="AC11" s="4"/>
+      <c r="AC11" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="AD11" s="4"/>
       <c r="AE11" s="4"/>
       <c r="AF11" s="4"/>
@@ -3374,7 +3420,7 @@
       <c r="T12" s="18">
         <v>96.5</v>
       </c>
-      <c r="U12" s="27" t="s">
+      <c r="U12" s="25" t="s">
         <v>595</v>
       </c>
       <c r="W12" s="2"/>
@@ -3383,9 +3429,11 @@
       </c>
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
-      <c r="AA12" s="26"/>
+      <c r="AA12" s="24"/>
       <c r="AB12" s="4"/>
-      <c r="AC12" s="4"/>
+      <c r="AC12" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="AD12" s="4"/>
       <c r="AE12" s="4"/>
       <c r="AF12" s="4"/>
@@ -3448,7 +3496,7 @@
       <c r="T13" s="18">
         <v>87.283363333333298</v>
       </c>
-      <c r="U13" s="27" t="s">
+      <c r="U13" s="25" t="s">
         <v>602</v>
       </c>
       <c r="W13" s="2"/>
@@ -3457,9 +3505,11 @@
       </c>
       <c r="Y13" s="4"/>
       <c r="Z13" s="4"/>
-      <c r="AA13" s="26"/>
+      <c r="AA13" s="24"/>
       <c r="AB13" s="4"/>
-      <c r="AC13" s="4"/>
+      <c r="AC13" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="AD13" s="4"/>
       <c r="AE13" s="4"/>
       <c r="AF13" s="4"/>
@@ -3522,7 +3572,7 @@
       <c r="T14" s="18">
         <v>87.952468181818105</v>
       </c>
-      <c r="U14" s="27" t="s">
+      <c r="U14" s="25" t="s">
         <v>595</v>
       </c>
       <c r="W14" s="2"/>
@@ -3531,9 +3581,11 @@
       </c>
       <c r="Y14" s="4"/>
       <c r="Z14" s="4"/>
-      <c r="AA14" s="26"/>
+      <c r="AA14" s="24"/>
       <c r="AB14" s="4"/>
-      <c r="AC14" s="4"/>
+      <c r="AC14" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="AD14" s="4"/>
       <c r="AE14" s="4"/>
       <c r="AF14" s="4"/>
@@ -3596,7 +3648,7 @@
       <c r="T15" s="18">
         <v>94.9796575757575</v>
       </c>
-      <c r="U15" s="27" t="s">
+      <c r="U15" s="25" t="s">
         <v>598</v>
       </c>
       <c r="W15" s="2"/>
@@ -3605,9 +3657,11 @@
       </c>
       <c r="Y15" s="4"/>
       <c r="Z15" s="4"/>
-      <c r="AA15" s="26"/>
+      <c r="AA15" s="24"/>
       <c r="AB15" s="4"/>
-      <c r="AC15" s="4"/>
+      <c r="AC15" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="AD15" s="4"/>
       <c r="AE15" s="4"/>
       <c r="AF15" s="4"/>
@@ -3668,8 +3722,8 @@
         <v>20</v>
       </c>
       <c r="T16" s="13"/>
-      <c r="U16" s="27"/>
-      <c r="V16" s="24" t="s">
+      <c r="U16" s="25"/>
+      <c r="V16" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W16" s="2"/>
@@ -3680,11 +3734,13 @@
       <c r="Z16" s="4">
         <v>2.4E-2</v>
       </c>
-      <c r="AA16" s="26" t="s">
-        <v>628</v>
+      <c r="AA16" s="24" t="s">
+        <v>627</v>
       </c>
       <c r="AB16" s="4"/>
-      <c r="AC16" s="4"/>
+      <c r="AC16" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="AD16" s="4"/>
       <c r="AE16" s="4"/>
       <c r="AF16" s="4"/>
@@ -3747,7 +3803,7 @@
       <c r="T17" s="18">
         <v>79.125</v>
       </c>
-      <c r="U17" s="27" t="s">
+      <c r="U17" s="25" t="s">
         <v>603</v>
       </c>
       <c r="W17" s="2"/>
@@ -3756,9 +3812,11 @@
       </c>
       <c r="Y17" s="4"/>
       <c r="Z17" s="4"/>
-      <c r="AA17" s="26"/>
+      <c r="AA17" s="24"/>
       <c r="AB17" s="4"/>
-      <c r="AC17" s="4"/>
+      <c r="AC17" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="AD17" s="4"/>
       <c r="AE17" s="4"/>
       <c r="AF17" s="4"/>
@@ -3821,7 +3879,7 @@
       <c r="T18" s="18">
         <v>94.185725000000005</v>
       </c>
-      <c r="U18" s="27" t="s">
+      <c r="U18" s="25" t="s">
         <v>598</v>
       </c>
       <c r="W18" s="2"/>
@@ -3830,9 +3888,11 @@
       </c>
       <c r="Y18" s="4"/>
       <c r="Z18" s="4"/>
-      <c r="AA18" s="26"/>
+      <c r="AA18" s="24"/>
       <c r="AB18" s="4"/>
-      <c r="AC18" s="4"/>
+      <c r="AC18" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="AD18" s="4"/>
       <c r="AE18" s="4"/>
       <c r="AF18" s="4"/>
@@ -3893,7 +3953,7 @@
       <c r="T19" s="18">
         <v>98.070440000000005</v>
       </c>
-      <c r="U19" s="27" t="s">
+      <c r="U19" s="25" t="s">
         <v>595</v>
       </c>
       <c r="W19" s="2"/>
@@ -3902,9 +3962,11 @@
       </c>
       <c r="Y19" s="4"/>
       <c r="Z19" s="4"/>
-      <c r="AA19" s="26"/>
+      <c r="AA19" s="24"/>
       <c r="AB19" s="4"/>
-      <c r="AC19" s="4"/>
+      <c r="AC19" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="AD19" s="4"/>
       <c r="AE19" s="4"/>
       <c r="AF19" s="4"/>
@@ -3965,25 +4027,27 @@
         <v>20</v>
       </c>
       <c r="T20" s="13"/>
-      <c r="U20" s="27"/>
-      <c r="V20" s="24" t="s">
+      <c r="U20" s="25"/>
+      <c r="V20" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W20" s="2"/>
-      <c r="X20" s="17" t="s">
+      <c r="X20" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="Y20" s="25" t="s">
+      <c r="Y20" s="4" t="s">
         <v>604</v>
       </c>
       <c r="Z20" s="4">
         <v>0.33300000000000002</v>
       </c>
-      <c r="AA20" s="26" t="s">
-        <v>629</v>
+      <c r="AA20" s="34" t="s">
+        <v>628</v>
       </c>
       <c r="AB20" s="4"/>
-      <c r="AC20" s="4"/>
+      <c r="AC20" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="AD20" s="4"/>
       <c r="AE20" s="4"/>
       <c r="AF20" s="4"/>
@@ -4046,7 +4110,7 @@
       <c r="T21" s="18">
         <v>87.143742857142797</v>
       </c>
-      <c r="U21" s="27" t="s">
+      <c r="U21" s="25" t="s">
         <v>596</v>
       </c>
       <c r="W21" s="2"/>
@@ -4055,9 +4119,11 @@
       </c>
       <c r="Y21" s="4"/>
       <c r="Z21" s="4"/>
-      <c r="AA21" s="26"/>
+      <c r="AA21" s="24"/>
       <c r="AB21" s="4"/>
-      <c r="AC21" s="4"/>
+      <c r="AC21" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="AD21" s="4"/>
       <c r="AE21" s="4"/>
       <c r="AF21" s="4"/>
@@ -4118,7 +4184,7 @@
       <c r="T22" s="18">
         <v>90.5</v>
       </c>
-      <c r="U22" s="27" t="s">
+      <c r="U22" s="25" t="s">
         <v>597</v>
       </c>
       <c r="W22" s="7"/>
@@ -4127,9 +4193,11 @@
       </c>
       <c r="Y22" s="4"/>
       <c r="Z22" s="4"/>
-      <c r="AA22" s="26"/>
+      <c r="AA22" s="24"/>
       <c r="AB22" s="4"/>
-      <c r="AC22" s="4"/>
+      <c r="AC22" s="6" t="s">
+        <v>149</v>
+      </c>
       <c r="AD22" s="4"/>
       <c r="AE22" s="4"/>
       <c r="AF22" s="4"/>
@@ -4190,7 +4258,7 @@
       <c r="T23" s="18">
         <v>85.789400000000001</v>
       </c>
-      <c r="U23" s="27" t="s">
+      <c r="U23" s="25" t="s">
         <v>602</v>
       </c>
       <c r="W23" s="2"/>
@@ -4199,9 +4267,11 @@
       </c>
       <c r="Y23" s="4"/>
       <c r="Z23" s="4"/>
-      <c r="AA23" s="26"/>
+      <c r="AA23" s="24"/>
       <c r="AB23" s="4"/>
-      <c r="AC23" s="4"/>
+      <c r="AC23" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="AD23" s="4"/>
       <c r="AE23" s="4"/>
       <c r="AF23" s="4"/>
@@ -4263,25 +4333,27 @@
       </c>
       <c r="S24" s="2"/>
       <c r="T24" s="13"/>
-      <c r="U24" s="27"/>
-      <c r="V24" s="24" t="s">
+      <c r="U24" s="25"/>
+      <c r="V24" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W24" s="2"/>
-      <c r="X24" s="2" t="s">
+      <c r="X24" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="Y24" s="25" t="s">
+      <c r="Y24" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="Z24" s="4">
+      <c r="Z24" s="33">
         <v>0.67200000000000004</v>
       </c>
-      <c r="AA24" s="26" t="s">
-        <v>630</v>
+      <c r="AA24" s="24" t="s">
+        <v>629</v>
       </c>
       <c r="AB24" s="4"/>
-      <c r="AC24" s="4"/>
+      <c r="AC24" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="AD24" s="4"/>
       <c r="AE24" s="4"/>
       <c r="AF24" s="4"/>
@@ -4342,7 +4414,7 @@
       <c r="T25" s="18">
         <v>86.129916666666603</v>
       </c>
-      <c r="U25" s="27" t="s">
+      <c r="U25" s="25" t="s">
         <v>606</v>
       </c>
       <c r="W25" s="2"/>
@@ -4351,9 +4423,11 @@
       </c>
       <c r="Y25" s="4"/>
       <c r="Z25" s="4"/>
-      <c r="AA25" s="26"/>
+      <c r="AA25" s="24"/>
       <c r="AB25" s="4"/>
-      <c r="AC25" s="4"/>
+      <c r="AC25" s="2" t="s">
+        <v>169</v>
+      </c>
       <c r="AD25" s="4"/>
       <c r="AE25" s="4"/>
       <c r="AF25" s="4"/>
@@ -4416,21 +4490,23 @@
       <c r="T26" s="22">
         <v>87.879083333333298</v>
       </c>
-      <c r="U26" s="27" t="s">
+      <c r="U26" s="25" t="s">
         <v>596</v>
       </c>
-      <c r="V26" s="23"/>
+      <c r="V26" s="14"/>
       <c r="W26" s="7"/>
       <c r="X26" s="7" t="s">
         <v>178</v>
       </c>
       <c r="Y26" s="4" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="Z26" s="4"/>
-      <c r="AA26" s="26"/>
+      <c r="AA26" s="24"/>
       <c r="AB26" s="4"/>
-      <c r="AC26" s="4"/>
+      <c r="AC26" s="7" t="s">
+        <v>175</v>
+      </c>
       <c r="AD26" s="4"/>
       <c r="AE26" s="4"/>
       <c r="AF26" s="4"/>
@@ -4493,7 +4569,7 @@
       <c r="T27" s="18">
         <v>89.519281300813006</v>
       </c>
-      <c r="U27" s="27" t="s">
+      <c r="U27" s="25" t="s">
         <v>601</v>
       </c>
       <c r="W27" s="2"/>
@@ -4502,9 +4578,11 @@
       </c>
       <c r="Y27" s="4"/>
       <c r="Z27" s="4"/>
-      <c r="AA27" s="26"/>
+      <c r="AA27" s="24"/>
       <c r="AB27" s="4"/>
-      <c r="AC27" s="4"/>
+      <c r="AC27" s="2" t="s">
+        <v>182</v>
+      </c>
       <c r="AD27" s="4"/>
       <c r="AE27" s="4"/>
       <c r="AF27" s="4"/>
@@ -4565,7 +4643,7 @@
       <c r="T28" s="18">
         <v>81.637972368421003</v>
       </c>
-      <c r="U28" s="27" t="s">
+      <c r="U28" s="25" t="s">
         <v>602</v>
       </c>
       <c r="W28" s="2"/>
@@ -4574,9 +4652,11 @@
       </c>
       <c r="Y28" s="4"/>
       <c r="Z28" s="4"/>
-      <c r="AA28" s="26"/>
+      <c r="AA28" s="24"/>
       <c r="AB28" s="4"/>
-      <c r="AC28" s="4"/>
+      <c r="AC28" s="2" t="s">
+        <v>188</v>
+      </c>
       <c r="AD28" s="4"/>
       <c r="AE28" s="4"/>
       <c r="AF28" s="4"/>
@@ -4637,7 +4717,7 @@
       <c r="T29" s="18">
         <v>87.276361904761899</v>
       </c>
-      <c r="U29" s="27" t="s">
+      <c r="U29" s="25" t="s">
         <v>602</v>
       </c>
       <c r="W29" s="2"/>
@@ -4646,9 +4726,11 @@
       </c>
       <c r="Y29" s="4"/>
       <c r="Z29" s="4"/>
-      <c r="AA29" s="26"/>
+      <c r="AA29" s="24"/>
       <c r="AB29" s="4"/>
-      <c r="AC29" s="4"/>
+      <c r="AC29" s="2" t="s">
+        <v>188</v>
+      </c>
       <c r="AD29" s="4"/>
       <c r="AE29" s="4"/>
       <c r="AF29" s="4"/>
@@ -4709,7 +4791,7 @@
       <c r="T30" s="18">
         <v>87.316566666666603</v>
       </c>
-      <c r="U30" s="27" t="s">
+      <c r="U30" s="25" t="s">
         <v>595</v>
       </c>
       <c r="W30" s="2"/>
@@ -4718,9 +4800,11 @@
       </c>
       <c r="Y30" s="4"/>
       <c r="Z30" s="4"/>
-      <c r="AA30" s="26"/>
+      <c r="AA30" s="24"/>
       <c r="AB30" s="4"/>
-      <c r="AC30" s="4"/>
+      <c r="AC30" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="AD30" s="4"/>
       <c r="AE30" s="4"/>
       <c r="AF30" s="4"/>
@@ -4783,7 +4867,7 @@
       <c r="T31" s="18">
         <v>86.888514285714294</v>
       </c>
-      <c r="U31" s="27" t="s">
+      <c r="U31" s="25" t="s">
         <v>596</v>
       </c>
       <c r="W31" s="2"/>
@@ -4792,9 +4876,11 @@
       </c>
       <c r="Y31" s="4"/>
       <c r="Z31" s="4"/>
-      <c r="AA31" s="26"/>
+      <c r="AA31" s="24"/>
       <c r="AB31" s="4"/>
-      <c r="AC31" s="4"/>
+      <c r="AC31" s="2" t="s">
+        <v>200</v>
+      </c>
       <c r="AD31" s="4"/>
       <c r="AE31" s="4"/>
       <c r="AF31" s="4"/>
@@ -4855,7 +4941,7 @@
       <c r="T32" s="18">
         <v>96.534666666666595</v>
       </c>
-      <c r="U32" s="27" t="s">
+      <c r="U32" s="25" t="s">
         <v>601</v>
       </c>
       <c r="W32" s="2"/>
@@ -4864,9 +4950,11 @@
       </c>
       <c r="Y32" s="4"/>
       <c r="Z32" s="4"/>
-      <c r="AA32" s="26"/>
+      <c r="AA32" s="24"/>
       <c r="AB32" s="4"/>
-      <c r="AC32" s="4"/>
+      <c r="AC32" s="2" t="s">
+        <v>206</v>
+      </c>
       <c r="AD32" s="4"/>
       <c r="AE32" s="4"/>
       <c r="AF32" s="4"/>
@@ -4928,8 +5016,8 @@
       </c>
       <c r="S33" s="2"/>
       <c r="T33" s="13"/>
-      <c r="U33" s="27"/>
-      <c r="V33" s="24" t="s">
+      <c r="U33" s="25"/>
+      <c r="V33" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W33" s="2"/>
@@ -4942,11 +5030,13 @@
       <c r="Z33" s="4">
         <v>0.11899999999999999</v>
       </c>
-      <c r="AA33" s="26" t="s">
-        <v>632</v>
+      <c r="AA33" s="24" t="s">
+        <v>631</v>
       </c>
       <c r="AB33" s="4"/>
-      <c r="AC33" s="4"/>
+      <c r="AC33" s="2" t="s">
+        <v>212</v>
+      </c>
       <c r="AD33" s="4"/>
       <c r="AE33" s="4"/>
       <c r="AF33" s="4"/>
@@ -5008,8 +5098,8 @@
       </c>
       <c r="S34" s="2"/>
       <c r="T34" s="13"/>
-      <c r="U34" s="27"/>
-      <c r="V34" s="24" t="s">
+      <c r="U34" s="25"/>
+      <c r="V34" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W34" s="2"/>
@@ -5020,11 +5110,13 @@
       <c r="Z34" s="4">
         <v>0.24</v>
       </c>
-      <c r="AA34" s="26" t="s">
-        <v>633</v>
+      <c r="AA34" s="24" t="s">
+        <v>632</v>
       </c>
       <c r="AB34" s="4"/>
-      <c r="AC34" s="4"/>
+      <c r="AC34" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="AD34" s="4"/>
       <c r="AE34" s="4"/>
       <c r="AF34" s="4"/>
@@ -5086,7 +5178,7 @@
       </c>
       <c r="S35" s="2"/>
       <c r="T35" s="13"/>
-      <c r="U35" s="27"/>
+      <c r="U35" s="25"/>
       <c r="V35" s="14" t="s">
         <v>607</v>
       </c>
@@ -5096,9 +5188,11 @@
       </c>
       <c r="Y35" s="4"/>
       <c r="Z35" s="4"/>
-      <c r="AA35" s="26"/>
+      <c r="AA35" s="24"/>
       <c r="AB35" s="4"/>
-      <c r="AC35" s="4"/>
+      <c r="AC35" s="2" t="s">
+        <v>220</v>
+      </c>
       <c r="AD35" s="4"/>
       <c r="AE35" s="4"/>
       <c r="AF35" s="4"/>
@@ -5160,8 +5254,8 @@
       </c>
       <c r="S36" s="2"/>
       <c r="T36" s="13"/>
-      <c r="U36" s="27"/>
-      <c r="V36" s="24" t="s">
+      <c r="U36" s="25"/>
+      <c r="V36" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W36" s="2"/>
@@ -5172,11 +5266,13 @@
       <c r="Z36" s="4">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="AA36" s="26" t="s">
-        <v>634</v>
+      <c r="AA36" s="24" t="s">
+        <v>633</v>
       </c>
       <c r="AB36" s="4"/>
-      <c r="AC36" s="4"/>
+      <c r="AC36" s="2" t="s">
+        <v>225</v>
+      </c>
       <c r="AD36" s="4"/>
       <c r="AE36" s="4"/>
       <c r="AF36" s="4"/>
@@ -5238,7 +5334,7 @@
       </c>
       <c r="S37" s="2"/>
       <c r="T37" s="13"/>
-      <c r="V37" s="24" t="s">
+      <c r="V37" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W37" s="2"/>
@@ -5249,11 +5345,13 @@
       <c r="Z37" s="4">
         <v>0.38100000000000001</v>
       </c>
-      <c r="AA37" s="26" t="s">
-        <v>635</v>
+      <c r="AA37" s="24" t="s">
+        <v>634</v>
       </c>
       <c r="AB37" s="4"/>
-      <c r="AC37" s="4"/>
+      <c r="AC37" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="AD37" s="4"/>
       <c r="AE37" s="4"/>
       <c r="AF37" s="4"/>
@@ -5315,7 +5413,7 @@
       </c>
       <c r="S38" s="2"/>
       <c r="T38" s="13"/>
-      <c r="V38" s="24" t="s">
+      <c r="V38" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W38" s="2"/>
@@ -5328,11 +5426,13 @@
       <c r="Z38" s="4">
         <v>0.27700000000000002</v>
       </c>
-      <c r="AA38" s="26" t="s">
-        <v>636</v>
+      <c r="AA38" s="24" t="s">
+        <v>635</v>
       </c>
       <c r="AB38" s="4"/>
-      <c r="AC38" s="4"/>
+      <c r="AC38" s="2" t="s">
+        <v>235</v>
+      </c>
       <c r="AD38" s="4"/>
       <c r="AE38" s="4"/>
       <c r="AF38" s="4"/>
@@ -5403,9 +5503,11 @@
       </c>
       <c r="Y39" s="4"/>
       <c r="Z39" s="4"/>
-      <c r="AA39" s="26"/>
+      <c r="AA39" s="24"/>
       <c r="AB39" s="4"/>
-      <c r="AC39" s="4"/>
+      <c r="AC39" s="2" t="s">
+        <v>240</v>
+      </c>
       <c r="AD39" s="4"/>
       <c r="AE39" s="4"/>
       <c r="AF39" s="4"/>
@@ -5467,24 +5569,26 @@
       </c>
       <c r="S40" s="2"/>
       <c r="T40" s="13"/>
-      <c r="V40" s="24" t="s">
+      <c r="V40" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W40" s="2"/>
       <c r="X40" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="Y40" s="25" t="s">
+      <c r="Y40" s="4" t="s">
         <v>611</v>
       </c>
       <c r="Z40" s="4">
         <v>0.33300000000000002</v>
       </c>
-      <c r="AA40" s="26" t="s">
-        <v>637</v>
+      <c r="AA40" s="24" t="s">
+        <v>636</v>
       </c>
       <c r="AB40" s="4"/>
-      <c r="AC40" s="4"/>
+      <c r="AC40" s="2" t="s">
+        <v>246</v>
+      </c>
       <c r="AD40" s="4"/>
       <c r="AE40" s="4"/>
       <c r="AF40" s="4"/>
@@ -5548,7 +5652,7 @@
       </c>
       <c r="S41" s="2"/>
       <c r="T41" s="13"/>
-      <c r="V41" s="24" t="s">
+      <c r="V41" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W41" s="2"/>
@@ -5559,9 +5663,11 @@
       <c r="Z41" s="4">
         <v>0</v>
       </c>
-      <c r="AA41" s="26"/>
+      <c r="AA41" s="24"/>
       <c r="AB41" s="4"/>
-      <c r="AC41" s="4"/>
+      <c r="AC41" s="2" t="s">
+        <v>251</v>
+      </c>
       <c r="AD41" s="4"/>
       <c r="AE41" s="4"/>
       <c r="AF41" s="4"/>
@@ -5634,9 +5740,11 @@
       </c>
       <c r="Y42" s="4"/>
       <c r="Z42" s="4"/>
-      <c r="AA42" s="26"/>
+      <c r="AA42" s="24"/>
       <c r="AB42" s="4"/>
-      <c r="AC42" s="4"/>
+      <c r="AC42" s="2" t="s">
+        <v>258</v>
+      </c>
       <c r="AD42" s="4"/>
       <c r="AE42" s="4"/>
       <c r="AF42" s="4"/>
@@ -5709,9 +5817,11 @@
       </c>
       <c r="Y43" s="4"/>
       <c r="Z43" s="4"/>
-      <c r="AA43" s="26"/>
+      <c r="AA43" s="24"/>
       <c r="AB43" s="4"/>
-      <c r="AC43" s="4"/>
+      <c r="AC43" s="2" t="s">
+        <v>266</v>
+      </c>
       <c r="AD43" s="4"/>
       <c r="AE43" s="4"/>
       <c r="AF43" s="4"/>
@@ -5775,7 +5885,7 @@
       </c>
       <c r="S44" s="2"/>
       <c r="T44" s="13"/>
-      <c r="V44" s="24" t="s">
+      <c r="V44" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W44" s="2"/>
@@ -5786,11 +5896,13 @@
       <c r="Z44" s="4">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="AA44" s="26" t="s">
-        <v>638</v>
+      <c r="AA44" s="24" t="s">
+        <v>637</v>
       </c>
       <c r="AB44" s="4"/>
-      <c r="AC44" s="4"/>
+      <c r="AC44" s="2" t="s">
+        <v>272</v>
+      </c>
       <c r="AD44" s="4"/>
       <c r="AE44" s="4"/>
       <c r="AF44" s="4"/>
@@ -5854,24 +5966,26 @@
       </c>
       <c r="S45" s="2"/>
       <c r="T45" s="13"/>
-      <c r="V45" s="24" t="s">
+      <c r="V45" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W45" s="2"/>
       <c r="X45" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="Y45" s="25" t="s">
+      <c r="Y45" s="4" t="s">
         <v>612</v>
       </c>
       <c r="Z45" s="4">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="AA45" s="26" t="s">
-        <v>639</v>
+      <c r="AA45" s="24" t="s">
+        <v>638</v>
       </c>
       <c r="AB45" s="4"/>
-      <c r="AC45" s="4"/>
+      <c r="AC45" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="AD45" s="4"/>
       <c r="AE45" s="4"/>
       <c r="AF45" s="4"/>
@@ -5944,9 +6058,11 @@
       </c>
       <c r="Y46" s="4"/>
       <c r="Z46" s="4"/>
-      <c r="AA46" s="26"/>
+      <c r="AA46" s="24"/>
       <c r="AB46" s="4"/>
-      <c r="AC46" s="4"/>
+      <c r="AC46" s="2" t="s">
+        <v>258</v>
+      </c>
       <c r="AD46" s="4"/>
       <c r="AE46" s="4"/>
       <c r="AF46" s="4"/>
@@ -6012,7 +6128,7 @@
       <c r="T47" s="15">
         <v>90.5</v>
       </c>
-      <c r="U47" s="27" t="s">
+      <c r="U47" s="25" t="s">
         <v>602</v>
       </c>
       <c r="W47" s="2"/>
@@ -6023,9 +6139,11 @@
         <v>613</v>
       </c>
       <c r="Z47" s="4"/>
-      <c r="AA47" s="26"/>
+      <c r="AA47" s="24"/>
       <c r="AB47" s="4"/>
-      <c r="AC47" s="4"/>
+      <c r="AC47" s="2" t="s">
+        <v>285</v>
+      </c>
       <c r="AD47" s="4"/>
       <c r="AE47" s="4"/>
       <c r="AF47" s="4"/>
@@ -6089,7 +6207,7 @@
       </c>
       <c r="S48" s="2"/>
       <c r="T48" s="13"/>
-      <c r="V48" s="24" t="s">
+      <c r="V48" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W48" s="2"/>
@@ -6100,11 +6218,13 @@
       <c r="Z48" s="4">
         <v>0.115</v>
       </c>
-      <c r="AA48" s="26" t="s">
-        <v>640</v>
+      <c r="AA48" s="24" t="s">
+        <v>639</v>
       </c>
       <c r="AB48" s="4"/>
-      <c r="AC48" s="4"/>
+      <c r="AC48" s="2" t="s">
+        <v>290</v>
+      </c>
       <c r="AD48" s="4"/>
       <c r="AE48" s="4"/>
       <c r="AF48" s="4"/>
@@ -6177,9 +6297,11 @@
       </c>
       <c r="Y49" s="4"/>
       <c r="Z49" s="4"/>
-      <c r="AA49" s="26"/>
+      <c r="AA49" s="24"/>
       <c r="AB49" s="4"/>
-      <c r="AC49" s="4"/>
+      <c r="AC49" s="2" t="s">
+        <v>295</v>
+      </c>
       <c r="AD49" s="4"/>
       <c r="AE49" s="4"/>
       <c r="AF49" s="4"/>
@@ -6243,7 +6365,7 @@
       </c>
       <c r="S50" s="2"/>
       <c r="T50" s="13"/>
-      <c r="V50" s="24" t="s">
+      <c r="V50" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W50" s="2"/>
@@ -6254,11 +6376,13 @@
       <c r="Z50" s="4">
         <v>0.14599999999999999</v>
       </c>
-      <c r="AA50" s="26" t="s">
-        <v>641</v>
+      <c r="AA50" s="24" t="s">
+        <v>640</v>
       </c>
       <c r="AB50" s="4"/>
-      <c r="AC50" s="4"/>
+      <c r="AC50" s="2" t="s">
+        <v>301</v>
+      </c>
       <c r="AD50" s="4"/>
       <c r="AE50" s="4"/>
       <c r="AF50" s="4"/>
@@ -6331,9 +6455,11 @@
       </c>
       <c r="Y51" s="4"/>
       <c r="Z51" s="4"/>
-      <c r="AA51" s="26"/>
+      <c r="AA51" s="24"/>
       <c r="AB51" s="4"/>
-      <c r="AC51" s="4"/>
+      <c r="AC51" s="2" t="s">
+        <v>308</v>
+      </c>
       <c r="AD51" s="4"/>
       <c r="AE51" s="4"/>
       <c r="AF51" s="4"/>
@@ -6396,7 +6522,7 @@
       </c>
       <c r="T52" s="19"/>
       <c r="U52" s="11"/>
-      <c r="V52" s="24" t="s">
+      <c r="V52" s="23" t="s">
         <v>608</v>
       </c>
       <c r="X52" s="10" t="s">
@@ -6408,11 +6534,13 @@
       <c r="Z52" s="4">
         <v>0.114</v>
       </c>
-      <c r="AA52" s="26" t="s">
-        <v>642</v>
+      <c r="AA52" s="24" t="s">
+        <v>641</v>
       </c>
       <c r="AB52" s="4"/>
-      <c r="AC52" s="4"/>
+      <c r="AC52" s="10" t="s">
+        <v>188</v>
+      </c>
       <c r="AD52" s="4"/>
       <c r="AE52" s="4"/>
       <c r="AF52" s="4"/>
@@ -6480,9 +6608,11 @@
       </c>
       <c r="Y53" s="4"/>
       <c r="Z53" s="4"/>
-      <c r="AA53" s="26"/>
+      <c r="AA53" s="24"/>
       <c r="AB53" s="4"/>
-      <c r="AC53" s="4"/>
+      <c r="AC53" s="10" t="s">
+        <v>235</v>
+      </c>
       <c r="AD53" s="4"/>
       <c r="AE53" s="4"/>
       <c r="AF53" s="4"/>
@@ -6555,9 +6685,11 @@
       </c>
       <c r="Y54" s="4"/>
       <c r="Z54" s="4"/>
-      <c r="AA54" s="26"/>
+      <c r="AA54" s="24"/>
       <c r="AB54" s="4"/>
-      <c r="AC54" s="4"/>
+      <c r="AC54" s="2" t="s">
+        <v>317</v>
+      </c>
       <c r="AD54" s="4"/>
       <c r="AE54" s="4"/>
       <c r="AF54" s="4"/>
@@ -6630,9 +6762,11 @@
       </c>
       <c r="Y55" s="4"/>
       <c r="Z55" s="4"/>
-      <c r="AA55" s="26"/>
+      <c r="AA55" s="24"/>
       <c r="AB55" s="4"/>
-      <c r="AC55" s="4"/>
+      <c r="AC55" s="2" t="s">
+        <v>323</v>
+      </c>
       <c r="AD55" s="4"/>
       <c r="AE55" s="4"/>
       <c r="AF55" s="4"/>
@@ -6705,9 +6839,11 @@
       </c>
       <c r="Y56" s="4"/>
       <c r="Z56" s="4"/>
-      <c r="AA56" s="26"/>
+      <c r="AA56" s="24"/>
       <c r="AB56" s="4"/>
-      <c r="AC56" s="4"/>
+      <c r="AC56" s="2" t="s">
+        <v>329</v>
+      </c>
       <c r="AD56" s="4"/>
       <c r="AE56" s="4"/>
       <c r="AF56" s="4"/>
@@ -6780,9 +6916,11 @@
       </c>
       <c r="Y57" s="4"/>
       <c r="Z57" s="4"/>
-      <c r="AA57" s="26"/>
+      <c r="AA57" s="24"/>
       <c r="AB57" s="4"/>
-      <c r="AC57" s="4"/>
+      <c r="AC57" s="2" t="s">
+        <v>337</v>
+      </c>
       <c r="AD57" s="4"/>
       <c r="AE57" s="4"/>
       <c r="AF57" s="4"/>
@@ -6846,7 +6984,7 @@
       </c>
       <c r="S58" s="2"/>
       <c r="T58" s="13"/>
-      <c r="V58" s="24" t="s">
+      <c r="V58" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W58" s="2"/>
@@ -6857,11 +6995,13 @@
       <c r="Z58" s="4">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="AA58" s="26" t="s">
-        <v>643</v>
+      <c r="AA58" s="24" t="s">
+        <v>642</v>
       </c>
       <c r="AB58" s="4"/>
-      <c r="AC58" s="4"/>
+      <c r="AC58" s="2" t="s">
+        <v>343</v>
+      </c>
       <c r="AD58" s="4"/>
       <c r="AE58" s="4"/>
       <c r="AF58" s="4"/>
@@ -6925,24 +7065,26 @@
       </c>
       <c r="S59" s="2"/>
       <c r="T59" s="13"/>
-      <c r="V59" s="24" t="s">
+      <c r="V59" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W59" s="2"/>
       <c r="X59" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="Y59" s="25" t="s">
+      <c r="Y59" s="4" t="s">
         <v>615</v>
       </c>
       <c r="Z59" s="4">
         <v>0.36099999999999999</v>
       </c>
-      <c r="AA59" s="26" t="s">
-        <v>644</v>
+      <c r="AA59" s="24" t="s">
+        <v>643</v>
       </c>
       <c r="AB59" s="4"/>
-      <c r="AC59" s="4"/>
+      <c r="AC59" s="2" t="s">
+        <v>349</v>
+      </c>
       <c r="AD59" s="4"/>
       <c r="AE59" s="4"/>
       <c r="AF59" s="4"/>
@@ -7015,9 +7157,11 @@
       </c>
       <c r="Y60" s="4"/>
       <c r="Z60" s="4"/>
-      <c r="AA60" s="26"/>
+      <c r="AA60" s="24"/>
       <c r="AB60" s="4"/>
-      <c r="AC60" s="4"/>
+      <c r="AC60" s="2" t="s">
+        <v>355</v>
+      </c>
       <c r="AD60" s="4"/>
       <c r="AE60" s="4"/>
       <c r="AF60" s="4"/>
@@ -7081,7 +7225,7 @@
       </c>
       <c r="S61" s="2"/>
       <c r="T61" s="13"/>
-      <c r="V61" s="24" t="s">
+      <c r="V61" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W61" s="2"/>
@@ -7092,11 +7236,13 @@
       <c r="Z61" s="4">
         <v>0.246</v>
       </c>
-      <c r="AA61" s="26" t="s">
-        <v>645</v>
+      <c r="AA61" s="24" t="s">
+        <v>644</v>
       </c>
       <c r="AB61" s="4"/>
-      <c r="AC61" s="4"/>
+      <c r="AC61" s="2" t="s">
+        <v>361</v>
+      </c>
       <c r="AD61" s="4"/>
       <c r="AE61" s="4"/>
       <c r="AF61" s="4"/>
@@ -7160,7 +7306,7 @@
       </c>
       <c r="S62" s="2"/>
       <c r="T62" s="13"/>
-      <c r="V62" s="24" t="s">
+      <c r="V62" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W62" s="2"/>
@@ -7171,11 +7317,13 @@
       <c r="Z62" s="4">
         <v>0.105</v>
       </c>
-      <c r="AA62" s="26" t="s">
-        <v>646</v>
+      <c r="AA62" s="24" t="s">
+        <v>645</v>
       </c>
       <c r="AB62" s="4"/>
-      <c r="AC62" s="4"/>
+      <c r="AC62" s="2" t="s">
+        <v>367</v>
+      </c>
       <c r="AD62" s="4"/>
       <c r="AE62" s="4"/>
       <c r="AF62" s="4"/>
@@ -7248,9 +7396,11 @@
       </c>
       <c r="Y63" s="4"/>
       <c r="Z63" s="4"/>
-      <c r="AA63" s="26"/>
+      <c r="AA63" s="24"/>
       <c r="AB63" s="4"/>
-      <c r="AC63" s="4"/>
+      <c r="AC63" s="2" t="s">
+        <v>371</v>
+      </c>
       <c r="AD63" s="4"/>
       <c r="AE63" s="4"/>
       <c r="AF63" s="4"/>
@@ -7314,7 +7464,7 @@
       </c>
       <c r="S64" s="2"/>
       <c r="T64" s="13"/>
-      <c r="V64" s="24" t="s">
+      <c r="V64" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W64" s="2"/>
@@ -7325,11 +7475,13 @@
       <c r="Z64" s="4">
         <v>0.3</v>
       </c>
-      <c r="AA64" s="26" t="s">
-        <v>632</v>
+      <c r="AA64" s="24" t="s">
+        <v>631</v>
       </c>
       <c r="AB64" s="4"/>
-      <c r="AC64" s="4"/>
+      <c r="AC64" s="2" t="s">
+        <v>376</v>
+      </c>
       <c r="AD64" s="4"/>
       <c r="AE64" s="4"/>
       <c r="AF64" s="4"/>
@@ -7402,9 +7554,11 @@
       </c>
       <c r="Y65" s="4"/>
       <c r="Z65" s="4"/>
-      <c r="AA65" s="26"/>
+      <c r="AA65" s="24"/>
       <c r="AB65" s="4"/>
-      <c r="AC65" s="4"/>
+      <c r="AC65" s="2" t="s">
+        <v>382</v>
+      </c>
       <c r="AD65" s="4"/>
       <c r="AE65" s="4"/>
       <c r="AF65" s="4"/>
@@ -7468,7 +7622,7 @@
       </c>
       <c r="S66" s="2"/>
       <c r="T66" s="13"/>
-      <c r="V66" s="24" t="s">
+      <c r="V66" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W66" s="2"/>
@@ -7479,11 +7633,13 @@
       <c r="Z66" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AA66" s="26" t="s">
-        <v>647</v>
+      <c r="AA66" s="24" t="s">
+        <v>646</v>
       </c>
       <c r="AB66" s="4"/>
-      <c r="AC66" s="4"/>
+      <c r="AC66" s="2" t="s">
+        <v>388</v>
+      </c>
       <c r="AD66" s="4"/>
       <c r="AE66" s="4"/>
       <c r="AF66" s="4"/>
@@ -7547,7 +7703,7 @@
       </c>
       <c r="S67" s="2"/>
       <c r="T67" s="13"/>
-      <c r="V67" s="24" t="s">
+      <c r="V67" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W67" s="2"/>
@@ -7558,11 +7714,13 @@
       <c r="Z67" s="4">
         <v>0.114</v>
       </c>
-      <c r="AA67" s="26" t="s">
-        <v>648</v>
+      <c r="AA67" s="24" t="s">
+        <v>647</v>
       </c>
       <c r="AB67" s="4"/>
-      <c r="AC67" s="4"/>
+      <c r="AC67" s="2" t="s">
+        <v>394</v>
+      </c>
       <c r="AD67" s="4"/>
       <c r="AE67" s="4"/>
       <c r="AF67" s="4"/>
@@ -7633,9 +7791,11 @@
       </c>
       <c r="Y68" s="4"/>
       <c r="Z68" s="4"/>
-      <c r="AA68" s="26"/>
+      <c r="AA68" s="24"/>
       <c r="AB68" s="4"/>
-      <c r="AC68" s="4"/>
+      <c r="AC68" s="2" t="s">
+        <v>400</v>
+      </c>
       <c r="AD68" s="4"/>
       <c r="AE68" s="4"/>
       <c r="AF68" s="4"/>
@@ -7706,9 +7866,11 @@
       </c>
       <c r="Y69" s="4"/>
       <c r="Z69" s="4"/>
-      <c r="AA69" s="26"/>
+      <c r="AA69" s="24"/>
       <c r="AB69" s="4"/>
-      <c r="AC69" s="4"/>
+      <c r="AC69" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="AD69" s="4"/>
       <c r="AE69" s="4"/>
       <c r="AF69" s="4"/>
@@ -7781,9 +7943,11 @@
       </c>
       <c r="Y70" s="4"/>
       <c r="Z70" s="4"/>
-      <c r="AA70" s="26"/>
+      <c r="AA70" s="24"/>
       <c r="AB70" s="4"/>
-      <c r="AC70" s="4"/>
+      <c r="AC70" s="2" t="s">
+        <v>412</v>
+      </c>
       <c r="AD70" s="4"/>
       <c r="AE70" s="4"/>
       <c r="AF70" s="4"/>
@@ -7856,9 +8020,11 @@
       </c>
       <c r="Y71" s="4"/>
       <c r="Z71" s="4"/>
-      <c r="AA71" s="26"/>
+      <c r="AA71" s="24"/>
       <c r="AB71" s="4"/>
-      <c r="AC71" s="4"/>
+      <c r="AC71" s="2" t="s">
+        <v>416</v>
+      </c>
       <c r="AD71" s="4"/>
       <c r="AE71" s="4"/>
       <c r="AF71" s="4"/>
@@ -7931,9 +8097,11 @@
       </c>
       <c r="Y72" s="4"/>
       <c r="Z72" s="4"/>
-      <c r="AA72" s="26"/>
+      <c r="AA72" s="24"/>
       <c r="AB72" s="4"/>
-      <c r="AC72" s="4"/>
+      <c r="AC72" s="2" t="s">
+        <v>421</v>
+      </c>
       <c r="AD72" s="4"/>
       <c r="AE72" s="4"/>
       <c r="AF72" s="4"/>
@@ -7993,7 +8161,7 @@
       </c>
       <c r="S73" s="2"/>
       <c r="T73" s="13"/>
-      <c r="V73" s="24" t="s">
+      <c r="V73" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W73" s="2"/>
@@ -8006,11 +8174,13 @@
       <c r="Z73" s="4">
         <v>0.38600000000000001</v>
       </c>
-      <c r="AA73" s="26" t="s">
-        <v>649</v>
+      <c r="AA73" s="24" t="s">
+        <v>648</v>
       </c>
       <c r="AB73" s="4"/>
-      <c r="AC73" s="4"/>
+      <c r="AC73" s="2" t="s">
+        <v>427</v>
+      </c>
       <c r="AD73" s="4"/>
       <c r="AE73" s="4"/>
       <c r="AF73" s="4"/>
@@ -8083,9 +8253,11 @@
       </c>
       <c r="Y74" s="4"/>
       <c r="Z74" s="4"/>
-      <c r="AA74" s="26"/>
+      <c r="AA74" s="24"/>
       <c r="AB74" s="4"/>
-      <c r="AC74" s="4"/>
+      <c r="AC74" s="2" t="s">
+        <v>433</v>
+      </c>
       <c r="AD74" s="4"/>
       <c r="AE74" s="4"/>
       <c r="AF74" s="4"/>
@@ -8158,9 +8330,11 @@
       </c>
       <c r="Y75" s="4"/>
       <c r="Z75" s="4"/>
-      <c r="AA75" s="26"/>
+      <c r="AA75" s="24"/>
       <c r="AB75" s="4"/>
-      <c r="AC75" s="4"/>
+      <c r="AC75" s="2" t="s">
+        <v>439</v>
+      </c>
       <c r="AD75" s="4"/>
       <c r="AE75" s="4"/>
       <c r="AF75" s="4"/>
@@ -8233,9 +8407,11 @@
       </c>
       <c r="Y76" s="4"/>
       <c r="Z76" s="4"/>
-      <c r="AA76" s="26"/>
+      <c r="AA76" s="24"/>
       <c r="AB76" s="4"/>
-      <c r="AC76" s="4"/>
+      <c r="AC76" s="2" t="s">
+        <v>446</v>
+      </c>
       <c r="AD76" s="4"/>
       <c r="AE76" s="4"/>
       <c r="AF76" s="4"/>
@@ -8299,7 +8475,7 @@
       </c>
       <c r="S77" s="2"/>
       <c r="T77" s="13"/>
-      <c r="V77" s="24" t="s">
+      <c r="V77" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W77" s="2"/>
@@ -8310,11 +8486,13 @@
       <c r="Z77" s="4">
         <v>0.161</v>
       </c>
-      <c r="AA77" s="26" t="s">
-        <v>650</v>
+      <c r="AA77" s="24" t="s">
+        <v>649</v>
       </c>
       <c r="AB77" s="4"/>
-      <c r="AC77" s="4"/>
+      <c r="AC77" s="2" t="s">
+        <v>452</v>
+      </c>
       <c r="AD77" s="4"/>
       <c r="AE77" s="4"/>
       <c r="AF77" s="4"/>
@@ -8380,7 +8558,7 @@
       <c r="T78" s="18">
         <v>74.0578</v>
       </c>
-      <c r="U78" s="27" t="s">
+      <c r="U78" s="25" t="s">
         <v>595</v>
       </c>
       <c r="W78" s="2"/>
@@ -8389,9 +8567,11 @@
       </c>
       <c r="Y78" s="4"/>
       <c r="Z78" s="4"/>
-      <c r="AA78" s="26"/>
+      <c r="AA78" s="24"/>
       <c r="AB78" s="4"/>
-      <c r="AC78" s="4"/>
+      <c r="AC78" s="2" t="s">
+        <v>458</v>
+      </c>
       <c r="AD78" s="4"/>
       <c r="AE78" s="4"/>
       <c r="AF78" s="4"/>
@@ -8464,9 +8644,11 @@
       </c>
       <c r="Y79" s="4"/>
       <c r="Z79" s="4"/>
-      <c r="AA79" s="26"/>
+      <c r="AA79" s="24"/>
       <c r="AB79" s="4"/>
-      <c r="AC79" s="4"/>
+      <c r="AC79" s="2" t="s">
+        <v>464</v>
+      </c>
       <c r="AD79" s="4"/>
       <c r="AE79" s="4"/>
       <c r="AF79" s="4"/>
@@ -8530,7 +8712,7 @@
       </c>
       <c r="S80" s="2"/>
       <c r="T80" s="13"/>
-      <c r="V80" s="24" t="s">
+      <c r="V80" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W80" s="2"/>
@@ -8541,11 +8723,13 @@
       <c r="Z80" s="4">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="AA80" s="26" t="s">
-        <v>651</v>
+      <c r="AA80" s="24" t="s">
+        <v>650</v>
       </c>
       <c r="AB80" s="4"/>
-      <c r="AC80" s="4"/>
+      <c r="AC80" s="2" t="s">
+        <v>470</v>
+      </c>
       <c r="AD80" s="4"/>
       <c r="AE80" s="4"/>
       <c r="AF80" s="4"/>
@@ -8609,7 +8793,7 @@
       </c>
       <c r="S81" s="2"/>
       <c r="T81" s="13"/>
-      <c r="V81" s="24" t="s">
+      <c r="V81" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W81" s="2"/>
@@ -8620,11 +8804,13 @@
       <c r="Z81" s="4">
         <v>0.17100000000000001</v>
       </c>
-      <c r="AA81" s="26" t="s">
-        <v>651</v>
+      <c r="AA81" s="24" t="s">
+        <v>650</v>
       </c>
       <c r="AB81" s="4"/>
-      <c r="AC81" s="4"/>
+      <c r="AC81" s="2" t="s">
+        <v>476</v>
+      </c>
       <c r="AD81" s="4"/>
       <c r="AE81" s="4"/>
       <c r="AF81" s="4"/>
@@ -8697,9 +8883,11 @@
       </c>
       <c r="Y82" s="4"/>
       <c r="Z82" s="4"/>
-      <c r="AA82" s="26"/>
+      <c r="AA82" s="24"/>
       <c r="AB82" s="4"/>
-      <c r="AC82" s="4"/>
+      <c r="AC82" s="2" t="s">
+        <v>480</v>
+      </c>
       <c r="AD82" s="4"/>
       <c r="AE82" s="4"/>
       <c r="AF82" s="4"/>
@@ -8772,9 +8960,11 @@
       </c>
       <c r="Y83" s="4"/>
       <c r="Z83" s="4"/>
-      <c r="AA83" s="26"/>
+      <c r="AA83" s="24"/>
       <c r="AB83" s="4"/>
-      <c r="AC83" s="4"/>
+      <c r="AC83" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="AD83" s="4"/>
       <c r="AE83" s="4"/>
       <c r="AF83" s="4"/>
@@ -8838,7 +9028,7 @@
       </c>
       <c r="S84" s="2"/>
       <c r="T84" s="13"/>
-      <c r="V84" s="24" t="s">
+      <c r="V84" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W84" s="2"/>
@@ -8849,11 +9039,13 @@
       <c r="Z84" s="4">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="AA84" s="26" t="s">
-        <v>652</v>
+      <c r="AA84" s="24" t="s">
+        <v>651</v>
       </c>
       <c r="AB84" s="4"/>
-      <c r="AC84" s="4"/>
+      <c r="AC84" s="2" t="s">
+        <v>491</v>
+      </c>
       <c r="AD84" s="4"/>
       <c r="AE84" s="4"/>
       <c r="AF84" s="4"/>
@@ -8926,9 +9118,11 @@
       </c>
       <c r="Y85" s="4"/>
       <c r="Z85" s="4"/>
-      <c r="AA85" s="26"/>
+      <c r="AA85" s="24"/>
       <c r="AB85" s="4"/>
-      <c r="AC85" s="4"/>
+      <c r="AC85" s="7" t="s">
+        <v>496</v>
+      </c>
       <c r="AD85" s="4"/>
       <c r="AE85" s="4"/>
       <c r="AF85" s="4"/>
@@ -9001,9 +9195,11 @@
       </c>
       <c r="Y86" s="4"/>
       <c r="Z86" s="4"/>
-      <c r="AA86" s="26"/>
+      <c r="AA86" s="24"/>
       <c r="AB86" s="4"/>
-      <c r="AC86" s="4"/>
+      <c r="AC86" s="7" t="s">
+        <v>503</v>
+      </c>
       <c r="AD86" s="4"/>
       <c r="AE86" s="4"/>
       <c r="AF86" s="4"/>
@@ -9074,9 +9270,11 @@
       </c>
       <c r="Y87" s="4"/>
       <c r="Z87" s="4"/>
-      <c r="AA87" s="26"/>
+      <c r="AA87" s="24"/>
       <c r="AB87" s="4"/>
-      <c r="AC87" s="4"/>
+      <c r="AC87" s="7" t="s">
+        <v>509</v>
+      </c>
       <c r="AD87" s="4"/>
       <c r="AE87" s="4"/>
       <c r="AF87" s="4"/>
@@ -9140,7 +9338,7 @@
       </c>
       <c r="S88" s="2"/>
       <c r="T88" s="20"/>
-      <c r="V88" s="24" t="s">
+      <c r="V88" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W88" s="7"/>
@@ -9148,14 +9346,16 @@
         <v>518</v>
       </c>
       <c r="Y88" s="4"/>
-      <c r="Z88" s="4">
+      <c r="Z88" s="33">
         <v>0.53100000000000003</v>
       </c>
-      <c r="AA88" s="26" t="s">
-        <v>653</v>
+      <c r="AA88" s="24" t="s">
+        <v>652</v>
       </c>
       <c r="AB88" s="4"/>
-      <c r="AC88" s="4"/>
+      <c r="AC88" s="7" t="s">
+        <v>515</v>
+      </c>
       <c r="AD88" s="4"/>
       <c r="AE88" s="4"/>
       <c r="AF88" s="4"/>
@@ -9226,9 +9426,11 @@
       </c>
       <c r="Y89" s="4"/>
       <c r="Z89" s="4"/>
-      <c r="AA89" s="26"/>
+      <c r="AA89" s="24"/>
       <c r="AB89" s="4"/>
-      <c r="AC89" s="4"/>
+      <c r="AC89" s="7" t="s">
+        <v>520</v>
+      </c>
       <c r="AD89" s="4"/>
       <c r="AE89" s="4"/>
       <c r="AF89" s="4"/>
@@ -9292,7 +9494,7 @@
       </c>
       <c r="S90" s="2"/>
       <c r="T90" s="20"/>
-      <c r="V90" s="24" t="s">
+      <c r="V90" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W90" s="7"/>
@@ -9303,11 +9505,13 @@
       <c r="Z90" s="4">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="AA90" s="26" t="s">
-        <v>654</v>
+      <c r="AA90" s="24" t="s">
+        <v>653</v>
       </c>
       <c r="AB90" s="4"/>
-      <c r="AC90" s="4"/>
+      <c r="AC90" s="7" t="s">
+        <v>526</v>
+      </c>
       <c r="AD90" s="4"/>
       <c r="AE90" s="4"/>
       <c r="AF90" s="4"/>
@@ -9380,9 +9584,11 @@
       </c>
       <c r="Y91" s="4"/>
       <c r="Z91" s="4"/>
-      <c r="AA91" s="26"/>
+      <c r="AA91" s="24"/>
       <c r="AB91" s="4"/>
-      <c r="AC91" s="4"/>
+      <c r="AC91" s="2" t="s">
+        <v>532</v>
+      </c>
       <c r="AD91" s="4"/>
       <c r="AE91" s="4"/>
       <c r="AF91" s="4"/>
@@ -9444,24 +9650,26 @@
       </c>
       <c r="S92" s="2"/>
       <c r="T92" s="13"/>
-      <c r="V92" s="24" t="s">
+      <c r="V92" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W92" s="2"/>
-      <c r="X92" s="17" t="s">
+      <c r="X92" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="Y92" s="25" t="s">
+      <c r="Y92" s="4" t="s">
         <v>618</v>
       </c>
       <c r="Z92" s="4">
         <v>0.217</v>
       </c>
-      <c r="AA92" s="26" t="s">
-        <v>655</v>
+      <c r="AA92" s="24" t="s">
+        <v>654</v>
       </c>
       <c r="AB92" s="4"/>
-      <c r="AC92" s="4"/>
+      <c r="AC92" s="2" t="s">
+        <v>382</v>
+      </c>
       <c r="AD92" s="4"/>
       <c r="AE92" s="4"/>
       <c r="AF92" s="4"/>
@@ -9530,9 +9738,11 @@
       </c>
       <c r="Y93" s="4"/>
       <c r="Z93" s="4"/>
-      <c r="AA93" s="26"/>
+      <c r="AA93" s="24"/>
       <c r="AB93" s="4"/>
-      <c r="AC93" s="4"/>
+      <c r="AC93" s="7" t="s">
+        <v>542</v>
+      </c>
       <c r="AD93" s="4"/>
       <c r="AE93" s="4"/>
       <c r="AF93" s="4"/>
@@ -9594,7 +9804,7 @@
       </c>
       <c r="S94" s="2"/>
       <c r="T94" s="20"/>
-      <c r="V94" s="24" t="s">
+      <c r="V94" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W94" s="7"/>
@@ -9605,11 +9815,13 @@
       <c r="Z94" s="4">
         <v>0.107</v>
       </c>
-      <c r="AA94" s="26" t="s">
-        <v>656</v>
+      <c r="AA94" s="24" t="s">
+        <v>655</v>
       </c>
       <c r="AB94" s="4"/>
-      <c r="AC94" s="4"/>
+      <c r="AC94" s="7" t="s">
+        <v>520</v>
+      </c>
       <c r="AD94" s="4"/>
       <c r="AE94" s="4"/>
       <c r="AF94" s="4"/>
@@ -9673,7 +9885,7 @@
       </c>
       <c r="S95" s="2"/>
       <c r="T95" s="13"/>
-      <c r="V95" s="24" t="s">
+      <c r="V95" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W95" s="2"/>
@@ -9684,11 +9896,13 @@
       <c r="Z95" s="4">
         <v>0.24299999999999999</v>
       </c>
-      <c r="AA95" s="26" t="s">
-        <v>657</v>
+      <c r="AA95" s="24" t="s">
+        <v>656</v>
       </c>
       <c r="AB95" s="4"/>
-      <c r="AC95" s="4"/>
+      <c r="AC95" s="2" t="s">
+        <v>550</v>
+      </c>
       <c r="AD95" s="4"/>
       <c r="AE95" s="4"/>
       <c r="AF95" s="4"/>
@@ -9761,9 +9975,11 @@
       </c>
       <c r="Y96" s="4"/>
       <c r="Z96" s="4"/>
-      <c r="AA96" s="26"/>
+      <c r="AA96" s="24"/>
       <c r="AB96" s="4"/>
-      <c r="AC96" s="4"/>
+      <c r="AC96" s="2" t="s">
+        <v>503</v>
+      </c>
       <c r="AD96" s="4"/>
       <c r="AE96" s="4"/>
       <c r="AF96" s="4"/>
@@ -9836,9 +10052,11 @@
       </c>
       <c r="Y97" s="4"/>
       <c r="Z97" s="4"/>
-      <c r="AA97" s="26"/>
+      <c r="AA97" s="24"/>
       <c r="AB97" s="4"/>
-      <c r="AC97" s="4"/>
+      <c r="AC97" s="2" t="s">
+        <v>559</v>
+      </c>
       <c r="AD97" s="4"/>
       <c r="AE97" s="4"/>
       <c r="AF97" s="4"/>
@@ -9902,7 +10120,7 @@
       </c>
       <c r="S98" s="2"/>
       <c r="T98" s="13"/>
-      <c r="V98" s="24" t="s">
+      <c r="V98" s="23" t="s">
         <v>608</v>
       </c>
       <c r="W98" s="2"/>
@@ -9913,11 +10131,13 @@
       <c r="Z98" s="4">
         <v>0.29599999999999999</v>
       </c>
-      <c r="AA98" s="26" t="s">
-        <v>658</v>
+      <c r="AA98" s="24" t="s">
+        <v>657</v>
       </c>
       <c r="AB98" s="4"/>
-      <c r="AC98" s="4"/>
+      <c r="AC98" s="2" t="s">
+        <v>565</v>
+      </c>
       <c r="AD98" s="4"/>
       <c r="AE98" s="4"/>
       <c r="AF98" s="4"/>
@@ -9990,9 +10210,11 @@
       </c>
       <c r="Y99" s="4"/>
       <c r="Z99" s="4"/>
-      <c r="AA99" s="26"/>
+      <c r="AA99" s="24"/>
       <c r="AB99" s="4"/>
-      <c r="AC99" s="4"/>
+      <c r="AC99" s="2" t="s">
+        <v>571</v>
+      </c>
       <c r="AD99" s="4"/>
       <c r="AE99" s="4"/>
       <c r="AF99" s="4"/>
@@ -10065,9 +10287,11 @@
       </c>
       <c r="Y100" s="4"/>
       <c r="Z100" s="4"/>
-      <c r="AA100" s="26"/>
+      <c r="AA100" s="24"/>
       <c r="AB100" s="4"/>
-      <c r="AC100" s="4"/>
+      <c r="AC100" s="2" t="s">
+        <v>577</v>
+      </c>
       <c r="AD100" s="4"/>
       <c r="AE100" s="4"/>
       <c r="AF100" s="4"/>
@@ -10133,20 +10357,22 @@
       <c r="T101" s="18">
         <v>97.091407692307698</v>
       </c>
-      <c r="U101" s="27" t="s">
+      <c r="U101" s="25" t="s">
         <v>601</v>
       </c>
       <c r="W101" s="2"/>
       <c r="X101" s="17" t="s">
         <v>586</v>
       </c>
-      <c r="Y101" s="25" t="s">
+      <c r="Y101" s="4" t="s">
         <v>619</v>
       </c>
       <c r="Z101" s="4"/>
-      <c r="AA101" s="26"/>
+      <c r="AA101" s="24"/>
       <c r="AB101" s="4"/>
-      <c r="AC101" s="4"/>
+      <c r="AC101" s="2" t="s">
+        <v>583</v>
+      </c>
       <c r="AD101" s="4"/>
       <c r="AE101" s="4"/>
       <c r="AF101" s="4"/>
@@ -10180,9 +10406,9 @@
       <c r="X102" s="2"/>
       <c r="Y102" s="4"/>
       <c r="Z102" s="4"/>
-      <c r="AA102" s="26"/>
+      <c r="AA102" s="24"/>
       <c r="AB102" s="4"/>
-      <c r="AC102" s="4"/>
+      <c r="AC102" s="2"/>
       <c r="AD102" s="4"/>
       <c r="AE102" s="4"/>
       <c r="AF102" s="4"/>
@@ -10196,9 +10422,8 @@
       <c r="H103" s="2"/>
       <c r="Y103" s="4"/>
       <c r="Z103" s="4"/>
-      <c r="AA103" s="26"/>
+      <c r="AA103" s="24"/>
       <c r="AB103" s="4"/>
-      <c r="AC103" s="4"/>
       <c r="AD103" s="4"/>
       <c r="AE103" s="4"/>
       <c r="AF103" s="4"/>
@@ -10210,9 +10435,8 @@
     <row r="104" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Y104" s="4"/>
       <c r="Z104" s="4"/>
-      <c r="AA104" s="26"/>
+      <c r="AA104" s="24"/>
       <c r="AB104" s="4"/>
-      <c r="AC104" s="4"/>
       <c r="AD104" s="4"/>
       <c r="AE104" s="4"/>
       <c r="AF104" s="4"/>
@@ -10224,9 +10448,8 @@
     <row r="105" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Y105" s="4"/>
       <c r="Z105" s="4"/>
-      <c r="AA105" s="26"/>
+      <c r="AA105" s="24"/>
       <c r="AB105" s="4"/>
-      <c r="AC105" s="4"/>
       <c r="AD105" s="4"/>
       <c r="AE105" s="4"/>
       <c r="AF105" s="4"/>
@@ -10239,9 +10462,8 @@
       <c r="V106" s="14"/>
       <c r="Y106" s="4"/>
       <c r="Z106" s="4"/>
-      <c r="AA106" s="26"/>
+      <c r="AA106" s="24"/>
       <c r="AB106" s="4"/>
-      <c r="AC106" s="4"/>
       <c r="AD106" s="4"/>
       <c r="AE106" s="4"/>
       <c r="AF106" s="4"/>
@@ -10258,9 +10480,8 @@
       <c r="X107" s="9"/>
       <c r="Y107" s="4"/>
       <c r="Z107" s="4"/>
-      <c r="AA107" s="26"/>
+      <c r="AA107" s="24"/>
       <c r="AB107" s="4"/>
-      <c r="AC107" s="4"/>
       <c r="AD107" s="4"/>
       <c r="AE107" s="4"/>
       <c r="AF107" s="4"/>
@@ -10272,9 +10493,8 @@
     <row r="108" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Y108" s="4"/>
       <c r="Z108" s="4"/>
-      <c r="AA108" s="26"/>
+      <c r="AA108" s="24"/>
       <c r="AB108" s="4"/>
-      <c r="AC108" s="4"/>
       <c r="AD108" s="4"/>
       <c r="AE108" s="4"/>
       <c r="AF108" s="4"/>
@@ -10290,9 +10510,8 @@
       <c r="X109" s="2"/>
       <c r="Y109" s="4"/>
       <c r="Z109" s="4"/>
-      <c r="AA109" s="26"/>
+      <c r="AA109" s="24"/>
       <c r="AB109" s="4"/>
-      <c r="AC109" s="4"/>
       <c r="AD109" s="4"/>
       <c r="AE109" s="4"/>
       <c r="AF109" s="4"/>
@@ -10302,72 +10521,72 @@
       <c r="AJ109" s="4"/>
     </row>
     <row r="110" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T110" s="28">
+      <c r="T110" s="26">
         <v>31</v>
       </c>
-      <c r="U110" s="32" t="s">
+      <c r="U110" s="30" t="s">
         <v>621</v>
       </c>
-      <c r="V110" s="29"/>
-      <c r="W110" s="29">
+      <c r="V110" s="27"/>
+      <c r="W110" s="27">
         <v>68</v>
       </c>
-      <c r="X110" s="29" t="s">
+      <c r="X110" s="27" t="s">
+        <v>658</v>
+      </c>
+      <c r="Y110" s="27"/>
+    </row>
+    <row r="111" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T111" s="26">
+        <v>30</v>
+      </c>
+      <c r="U111" s="30" t="s">
+        <v>620</v>
+      </c>
+      <c r="V111" s="27"/>
+      <c r="W111" s="27">
+        <v>35</v>
+      </c>
+      <c r="X111" s="27" t="s">
+        <v>607</v>
+      </c>
+      <c r="Y111" s="27"/>
+    </row>
+    <row r="112" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T112" s="26">
+        <v>1</v>
+      </c>
+      <c r="U112" s="30" t="s">
+        <v>622</v>
+      </c>
+      <c r="V112" s="27"/>
+      <c r="W112" s="27">
+        <v>32</v>
+      </c>
+      <c r="X112" s="27" t="s">
+        <v>608</v>
+      </c>
+      <c r="Y112" s="27"/>
+    </row>
+    <row r="113" spans="8:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T113" s="26"/>
+      <c r="U113" s="30"/>
+      <c r="V113" s="27"/>
+      <c r="W113" s="27">
+        <v>1</v>
+      </c>
+      <c r="X113" s="27" t="s">
         <v>623</v>
       </c>
-      <c r="Y110" s="29"/>
-    </row>
-    <row r="111" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T111" s="28">
-        <v>30</v>
-      </c>
-      <c r="U111" s="32" t="s">
-        <v>620</v>
-      </c>
-      <c r="V111" s="29"/>
-      <c r="W111" s="29">
-        <v>35</v>
-      </c>
-      <c r="X111" s="29" t="s">
-        <v>607</v>
-      </c>
-      <c r="Y111" s="29"/>
-    </row>
-    <row r="112" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T112" s="28">
-        <v>1</v>
-      </c>
-      <c r="U112" s="32" t="s">
-        <v>622</v>
-      </c>
-      <c r="V112" s="29"/>
-      <c r="W112" s="29">
-        <v>32</v>
-      </c>
-      <c r="X112" s="29" t="s">
-        <v>608</v>
-      </c>
-      <c r="Y112" s="29"/>
-    </row>
-    <row r="113" spans="8:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T113" s="28"/>
-      <c r="U113" s="32"/>
-      <c r="V113" s="29"/>
-      <c r="W113" s="29">
-        <v>1</v>
-      </c>
-      <c r="X113" s="29" t="s">
-        <v>624</v>
-      </c>
-      <c r="Y113" s="29"/>
+      <c r="Y113" s="27"/>
     </row>
     <row r="114" spans="8:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T114" s="28"/>
-      <c r="U114" s="32"/>
-      <c r="V114" s="29"/>
-      <c r="W114" s="29"/>
-      <c r="X114" s="29"/>
-      <c r="Y114" s="29"/>
+      <c r="T114" s="26"/>
+      <c r="U114" s="30"/>
+      <c r="V114" s="27"/>
+      <c r="W114" s="27"/>
+      <c r="X114" s="27"/>
+      <c r="Y114" s="27"/>
     </row>
     <row r="125" spans="8:25" ht="13" x14ac:dyDescent="0.15">
       <c r="H125" s="2" t="s">
@@ -10472,5 +10691,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>